<commit_message>
several fixes in Importer
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_first.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_first.xlsx
@@ -20,12 +20,12 @@
     <definedName name="Treatment">LookUp!$C$2:$C$11</definedName>
     <definedName name="Units">LookUp!$D$2:$D$32</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Product Name</t>
   </si>
@@ -231,21 +231,9 @@
     <t>Ultra Heating</t>
   </si>
   <si>
-    <t>"Pflicht"-Felder</t>
-  </si>
-  <si>
-    <t>unterstrichen!</t>
-  </si>
-  <si>
-    <t>muss ausgefüllt werden vom Inspektor</t>
-  </si>
-  <si>
     <t>Sampling</t>
   </si>
   <si>
-    <t>IMMER echte PFLICHT!!! Falls nicht bekannt, dann bitte eines ausdenken!</t>
-  </si>
-  <si>
     <t>Station</t>
   </si>
   <si>
@@ -334,6 +322,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Best before date</t>
+  </si>
+  <si>
+    <t>Must be filled in / must be checked by inspector</t>
+  </si>
+  <si>
+    <t>are underlined</t>
+  </si>
+  <si>
+    <t>ALWAYS MANDATORY!!! Please create a lot number if the true number is unknown.</t>
+  </si>
+  <si>
+    <t>Every DeliveryID MUST BE UNIQUE! Apart from this any ID can be used: Words, numbers, formulas (e.g. "=B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;G3&amp;"."&amp;H3&amp;"."&amp;I3&amp;";"&amp;O3")</t>
+  </si>
+  <si>
+    <t>Mandatory fields</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -623,31 +626,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -669,6 +647,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,6 +674,27 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1025,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>6</v>
@@ -1043,7 +1049,7 @@
         <v>10</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
@@ -1106,123 +1112,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="30"/>
+      <c r="O1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="V1" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+    </row>
+    <row r="2" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="W1" s="25" t="s">
+      <c r="G2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-    </row>
-    <row r="2" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>79</v>
-      </c>
       <c r="N2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
+        <v>73</v>
+      </c>
+      <c r="O2" s="28"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1234,18 +1252,6 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576 M3:M1048576">
@@ -1298,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>24</v>
@@ -1315,7 +1321,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>67</v>
@@ -1329,7 +1335,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>66</v>
@@ -1343,7 +1349,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>59</v>
@@ -1357,7 +1363,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>65</v>
@@ -1371,7 +1377,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>60</v>
@@ -1385,7 +1391,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -1399,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>61</v>
@@ -1413,7 +1419,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>62</v>
@@ -1427,7 +1433,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>63</v>
@@ -1441,7 +1447,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>64</v>
@@ -1571,7 +1577,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1584,15 +1590,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>103</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,7 +1606,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
krisenimporter updated - fin
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_first.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_first.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
   <si>
     <t>Product Name</t>
   </si>
@@ -312,15 +312,6 @@
     <t>DeliveryID</t>
   </si>
   <si>
-    <t>Production date Day</t>
-  </si>
-  <si>
-    <t>Production date Month</t>
-  </si>
-  <si>
-    <t>Production date Year</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Best before date</t>
   </si>
   <si>
@@ -337,6 +328,9 @@
   </si>
   <si>
     <t>Mandatory fields</t>
+  </si>
+  <si>
+    <t>Production date</t>
   </si>
 </sst>
 </file>
@@ -458,7 +452,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -518,26 +512,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -626,6 +607,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -647,13 +649,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -674,27 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1077,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A2"/>
@@ -1101,86 +1075,76 @@
     <col min="14" max="14" width="12.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="39.42578125" style="2" customWidth="1"/>
     <col min="16" max="16" width="10" style="12" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="21" style="2" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" style="2" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="19" width="10.5703125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="21" style="2" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:27" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="29" t="s">
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="27" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="S1" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="T1" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="U1" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="V1" s="31" t="s">
+      <c r="T1" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="W1" s="41" t="s">
+      <c r="U1" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-    </row>
-    <row r="2" spans="1:29" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+    </row>
+    <row r="2" spans="1:27" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="24" t="s">
         <v>75</v>
       </c>
@@ -1211,36 +1175,24 @@
       <c r="N2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="28"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="40"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="Z1:Z2"/>
+  <mergeCells count="21">
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1252,20 +1204,28 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="X1:X2"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576 M3:M1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U1048576 R3:R1048576 G3:G1048576 J3:J1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576 J3:J1048576">
       <formula1>1</formula1>
       <formula2>31</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:S1048576 H3:H1048576 K3:K1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576 K3:K1048576">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576 I3:I1048576 L3:L1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I1048576 L3:L1048576">
       <formula1>1900</formula1>
       <formula2>3000</formula2>
     </dataValidation>
@@ -1275,10 +1235,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N1048576 F3:F1048576">
       <formula1>Units</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T3:T1048576">
       <formula1>Treatment</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U1048576">
       <formula1>Sampling</formula1>
     </dataValidation>
   </dataValidations>
@@ -1590,15 +1550,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="44" t="s">
         <v>100</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1606,7 +1566,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1574,7 @@
         <v>94</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>